<commit_message>
time between injuries complete
</commit_message>
<xml_diff>
--- a/sims_data_1.xlsx
+++ b/sims_data_1.xlsx
@@ -833,7 +833,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -1263,12 +1263,12 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
@@ -1351,12 +1351,12 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
@@ -1693,12 +1693,12 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
@@ -1781,7 +1781,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -2196,7 +2196,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -2284,12 +2284,12 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
@@ -2855,7 +2855,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -2943,7 +2943,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -3031,12 +3031,12 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
@@ -3592,7 +3592,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
@@ -3929,7 +3929,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
@@ -4017,12 +4017,12 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
@@ -4105,7 +4105,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -4271,7 +4271,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -4437,7 +4437,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
@@ -4525,7 +4525,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -4613,12 +4613,12 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
@@ -4935,12 +4935,12 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L55" t="inlineStr">
@@ -5277,12 +5277,12 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L59" t="inlineStr">
@@ -5360,12 +5360,12 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L60" t="inlineStr">
@@ -5443,12 +5443,12 @@
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L61" t="inlineStr">
@@ -5599,12 +5599,12 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L63" t="inlineStr">
@@ -5765,7 +5765,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
@@ -5931,12 +5931,12 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L67" t="inlineStr">
@@ -6024,7 +6024,7 @@
       </c>
       <c r="K68" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L68" t="inlineStr">
@@ -6107,12 +6107,12 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L69" t="inlineStr">
@@ -6190,7 +6190,7 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
@@ -6542,7 +6542,7 @@
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K74" t="inlineStr">
@@ -6630,7 +6630,7 @@
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L75" t="inlineStr">
@@ -6708,12 +6708,12 @@
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L76" t="inlineStr">
@@ -6791,12 +6791,12 @@
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K77" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L77" t="inlineStr">
@@ -7485,12 +7485,12 @@
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K85" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L85" t="inlineStr">
@@ -7573,12 +7573,12 @@
       </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K86" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L86" t="inlineStr">
@@ -7661,12 +7661,12 @@
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K87" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L87" t="inlineStr">
@@ -8257,12 +8257,12 @@
       </c>
       <c r="J94" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K94" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L94" t="inlineStr">
@@ -8345,12 +8345,12 @@
       </c>
       <c r="J95" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K95" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L95" t="inlineStr">
@@ -8755,12 +8755,12 @@
       </c>
       <c r="J100" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K100" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L100" t="inlineStr">
@@ -9019,12 +9019,12 @@
       </c>
       <c r="J103" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K103" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L103" t="inlineStr">
@@ -9414,12 +9414,12 @@
       </c>
       <c r="J108" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K108" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L108" t="inlineStr">
@@ -9502,12 +9502,12 @@
       </c>
       <c r="J109" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K109" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L109" t="inlineStr">
@@ -9590,12 +9590,12 @@
       </c>
       <c r="J110" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K110" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L110" t="inlineStr">
@@ -9683,7 +9683,7 @@
       </c>
       <c r="K111" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L111" t="inlineStr">
@@ -9766,12 +9766,12 @@
       </c>
       <c r="J112" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K112" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L112" t="inlineStr">
@@ -10284,7 +10284,7 @@
       </c>
       <c r="J118" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K118" t="inlineStr">
@@ -10372,12 +10372,12 @@
       </c>
       <c r="J119" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K119" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L119" t="inlineStr">
@@ -11146,12 +11146,12 @@
       </c>
       <c r="J129" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K129" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L129" t="inlineStr">
@@ -11234,12 +11234,12 @@
       </c>
       <c r="J130" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K130" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L130" t="inlineStr">
@@ -11327,7 +11327,7 @@
       </c>
       <c r="K131" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L131" t="inlineStr">
@@ -11498,7 +11498,7 @@
       </c>
       <c r="J133" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K133" t="inlineStr">
@@ -11591,7 +11591,7 @@
       </c>
       <c r="K134" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L134" t="inlineStr">
@@ -11669,12 +11669,12 @@
       </c>
       <c r="J135" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K135" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L135" t="inlineStr">
@@ -11752,12 +11752,12 @@
       </c>
       <c r="J136" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K136" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L136" t="inlineStr">
@@ -11918,12 +11918,12 @@
       </c>
       <c r="J138" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K138" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L138" t="inlineStr">
@@ -12069,12 +12069,12 @@
       </c>
       <c r="J140" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K140" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L140" t="inlineStr">
@@ -12323,7 +12323,7 @@
       </c>
       <c r="J143" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K143" t="inlineStr">
@@ -12411,12 +12411,12 @@
       </c>
       <c r="J144" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K144" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L144" t="inlineStr">
@@ -12748,12 +12748,12 @@
       </c>
       <c r="J148" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K148" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L148" t="inlineStr">
@@ -12836,12 +12836,12 @@
       </c>
       <c r="J149" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K149" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L149" t="inlineStr">
@@ -13261,7 +13261,7 @@
       </c>
       <c r="J154" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K154" t="inlineStr">
@@ -13349,12 +13349,12 @@
       </c>
       <c r="J155" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K155" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L155" t="inlineStr">
@@ -13437,7 +13437,7 @@
       </c>
       <c r="J156" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K156" t="inlineStr">
@@ -13525,7 +13525,7 @@
       </c>
       <c r="J157" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K157" t="inlineStr">
@@ -13613,12 +13613,12 @@
       </c>
       <c r="J158" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K158" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L158" t="inlineStr">
@@ -13789,12 +13789,12 @@
       </c>
       <c r="J160" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K160" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L160" t="inlineStr">
@@ -14277,12 +14277,12 @@
       </c>
       <c r="J166" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K166" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L166" t="inlineStr">
@@ -14360,12 +14360,12 @@
       </c>
       <c r="J167" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K167" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L167" t="inlineStr">
@@ -14785,12 +14785,12 @@
       </c>
       <c r="J172" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K172" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L172" t="inlineStr">
@@ -14951,12 +14951,12 @@
       </c>
       <c r="J174" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K174" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L174" t="inlineStr">
@@ -15449,12 +15449,12 @@
       </c>
       <c r="J180" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K180" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L180" t="inlineStr">
@@ -15532,12 +15532,12 @@
       </c>
       <c r="J181" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K181" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L181" t="inlineStr">
@@ -15688,12 +15688,12 @@
       </c>
       <c r="J183" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K183" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L183" t="inlineStr">
@@ -15776,12 +15776,12 @@
       </c>
       <c r="J184" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K184" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L184" t="inlineStr">
@@ -16010,12 +16010,12 @@
       </c>
       <c r="J187" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K187" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L187" t="inlineStr">
@@ -16171,12 +16171,12 @@
       </c>
       <c r="J189" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K189" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L189" t="inlineStr">
@@ -16259,12 +16259,12 @@
       </c>
       <c r="J190" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K190" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L190" t="inlineStr">
@@ -16425,12 +16425,12 @@
       </c>
       <c r="J192" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K192" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L192" t="inlineStr">
@@ -16513,7 +16513,7 @@
       </c>
       <c r="J193" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K193" t="inlineStr">
@@ -16782,7 +16782,7 @@
       </c>
       <c r="K196" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L196" t="inlineStr">
@@ -16953,12 +16953,12 @@
       </c>
       <c r="J198" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K198" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L198" t="inlineStr">
@@ -17041,12 +17041,12 @@
       </c>
       <c r="J199" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K199" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L199" t="inlineStr">
@@ -17129,12 +17129,12 @@
       </c>
       <c r="J200" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K200" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L200" t="inlineStr">
@@ -17383,7 +17383,7 @@
       </c>
       <c r="J203" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K203" t="inlineStr">
@@ -17471,12 +17471,12 @@
       </c>
       <c r="J204" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K204" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L204" t="inlineStr">
@@ -17803,12 +17803,12 @@
       </c>
       <c r="J208" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K208" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L208" t="inlineStr">
@@ -18057,7 +18057,7 @@
       </c>
       <c r="J211" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K211" t="inlineStr">
@@ -18145,12 +18145,12 @@
       </c>
       <c r="J212" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K212" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L212" t="inlineStr">
@@ -18394,12 +18394,12 @@
       </c>
       <c r="J215" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K215" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L215" t="inlineStr">
@@ -18482,12 +18482,12 @@
       </c>
       <c r="J216" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K216" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L216" t="inlineStr">
@@ -18663,7 +18663,7 @@
       </c>
       <c r="K218" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L218" t="inlineStr">
@@ -18751,7 +18751,7 @@
       </c>
       <c r="K219" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L219" t="inlineStr">
@@ -19073,12 +19073,12 @@
       </c>
       <c r="J223" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K223" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L223" t="inlineStr">
@@ -19156,7 +19156,7 @@
       </c>
       <c r="J224" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K224" t="inlineStr">
@@ -19410,7 +19410,7 @@
       </c>
       <c r="J227" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K227" t="inlineStr">
@@ -19586,12 +19586,12 @@
       </c>
       <c r="J229" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K229" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L229" t="inlineStr">
@@ -19830,12 +19830,12 @@
       </c>
       <c r="J232" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K232" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L232" t="inlineStr">
@@ -20099,7 +20099,7 @@
       </c>
       <c r="K235" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L235" t="inlineStr">
@@ -20421,12 +20421,12 @@
       </c>
       <c r="J239" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K239" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L239" t="inlineStr">
@@ -20509,12 +20509,12 @@
       </c>
       <c r="J240" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K240" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L240" t="inlineStr">
@@ -20690,7 +20690,7 @@
       </c>
       <c r="K242" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L242" t="inlineStr">
@@ -20773,12 +20773,12 @@
       </c>
       <c r="J243" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K243" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L243" t="inlineStr">
@@ -21324,12 +21324,12 @@
       </c>
       <c r="J250" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K250" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L250" t="inlineStr">
@@ -21572,12 +21572,12 @@
       </c>
       <c r="J253" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K253" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L253" t="inlineStr">
@@ -21665,7 +21665,7 @@
       </c>
       <c r="K254" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L254" t="inlineStr">
@@ -21748,12 +21748,12 @@
       </c>
       <c r="J255" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K255" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L255" t="inlineStr">
@@ -22012,12 +22012,12 @@
       </c>
       <c r="J258" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K258" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L258" t="inlineStr">
@@ -22095,12 +22095,12 @@
       </c>
       <c r="J259" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K259" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L259" t="inlineStr">
@@ -22417,12 +22417,12 @@
       </c>
       <c r="J263" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K263" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L263" t="inlineStr">
@@ -22505,12 +22505,12 @@
       </c>
       <c r="J264" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K264" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L264" t="inlineStr">
@@ -23315,12 +23315,12 @@
       </c>
       <c r="J274" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K274" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L274" t="inlineStr">
@@ -24097,7 +24097,7 @@
       </c>
       <c r="J283" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K283" t="inlineStr">
@@ -24185,7 +24185,7 @@
       </c>
       <c r="J284" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K284" t="inlineStr">
@@ -24693,12 +24693,12 @@
       </c>
       <c r="J290" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K290" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L290" t="inlineStr">
@@ -24859,12 +24859,12 @@
       </c>
       <c r="J292" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K292" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L292" t="inlineStr">
@@ -24947,12 +24947,12 @@
       </c>
       <c r="J293" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K293" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L293" t="inlineStr">
@@ -25035,12 +25035,12 @@
       </c>
       <c r="J294" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K294" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L294" t="inlineStr">
@@ -25123,12 +25123,12 @@
       </c>
       <c r="J295" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K295" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L295" t="inlineStr">
@@ -25805,7 +25805,7 @@
       </c>
       <c r="J304" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K304" t="inlineStr">
@@ -25893,12 +25893,12 @@
       </c>
       <c r="J305" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K305" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L305" t="inlineStr">
@@ -26069,12 +26069,12 @@
       </c>
       <c r="J307" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K307" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L307" t="inlineStr">
@@ -26157,7 +26157,7 @@
       </c>
       <c r="J308" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K308" t="inlineStr">
@@ -26245,12 +26245,12 @@
       </c>
       <c r="J309" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K309" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L309" t="inlineStr">
@@ -26333,12 +26333,12 @@
       </c>
       <c r="J310" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K310" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L310" t="inlineStr">
@@ -26597,12 +26597,12 @@
       </c>
       <c r="J313" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K313" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L313" t="inlineStr">
@@ -26685,12 +26685,12 @@
       </c>
       <c r="J314" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K314" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L314" t="inlineStr">
@@ -26773,12 +26773,12 @@
       </c>
       <c r="J315" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K315" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L315" t="inlineStr">
@@ -26861,12 +26861,12 @@
       </c>
       <c r="J316" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K316" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L316" t="inlineStr">
@@ -27203,7 +27203,7 @@
       </c>
       <c r="J320" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K320" t="inlineStr">
@@ -27291,12 +27291,12 @@
       </c>
       <c r="J321" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K321" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L321" t="inlineStr">
@@ -27379,12 +27379,12 @@
       </c>
       <c r="J322" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K322" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L322" t="inlineStr">
@@ -27549,7 +27549,7 @@
       </c>
       <c r="J324" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K324" t="inlineStr">
@@ -27818,7 +27818,7 @@
       </c>
       <c r="K327" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L327" t="inlineStr">
@@ -27901,12 +27901,12 @@
       </c>
       <c r="J328" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K328" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L328" t="inlineStr">
@@ -27983,12 +27983,12 @@
       </c>
       <c r="J329" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K329" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L329" t="inlineStr">
@@ -28516,7 +28516,7 @@
       </c>
       <c r="K335" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L335" t="inlineStr">
@@ -28951,12 +28951,12 @@
       </c>
       <c r="J340" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K340" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L340" t="inlineStr">
@@ -29034,12 +29034,12 @@
       </c>
       <c r="J341" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K341" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L341" t="inlineStr">
@@ -29386,12 +29386,12 @@
       </c>
       <c r="J345" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K345" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L345" t="inlineStr">
@@ -29474,12 +29474,12 @@
       </c>
       <c r="J346" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K346" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L346" t="inlineStr">
@@ -29650,12 +29650,12 @@
       </c>
       <c r="J348" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K348" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L348" t="inlineStr">
@@ -29738,12 +29738,12 @@
       </c>
       <c r="J349" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K349" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L349" t="inlineStr">
@@ -29826,12 +29826,12 @@
       </c>
       <c r="J350" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K350" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L350" t="inlineStr">
@@ -29914,7 +29914,7 @@
       </c>
       <c r="J351" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K351" t="inlineStr">
@@ -30090,12 +30090,12 @@
       </c>
       <c r="J353" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K353" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L353" t="inlineStr">
@@ -30266,12 +30266,12 @@
       </c>
       <c r="J355" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K355" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L355" t="inlineStr">
@@ -30432,12 +30432,12 @@
       </c>
       <c r="J357" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K357" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L357" t="inlineStr">
@@ -30769,12 +30769,12 @@
       </c>
       <c r="J361" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K361" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L361" t="inlineStr">
@@ -30857,7 +30857,7 @@
       </c>
       <c r="J362" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K362" t="inlineStr">
@@ -31277,12 +31277,12 @@
       </c>
       <c r="J367" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K367" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L367" t="inlineStr">
@@ -31365,7 +31365,7 @@
       </c>
       <c r="J368" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K368" t="inlineStr">
@@ -31453,12 +31453,12 @@
       </c>
       <c r="J369" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K369" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L369" t="inlineStr">
@@ -31536,12 +31536,12 @@
       </c>
       <c r="J370" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K370" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L370" t="inlineStr">
@@ -31624,12 +31624,12 @@
       </c>
       <c r="J371" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K371" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L371" t="inlineStr">
@@ -31707,7 +31707,7 @@
       </c>
       <c r="J372" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K372" t="inlineStr">
@@ -31790,7 +31790,7 @@
       </c>
       <c r="J373" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K373" t="inlineStr">
@@ -32220,12 +32220,12 @@
       </c>
       <c r="J378" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K378" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L378" t="inlineStr">
@@ -32308,7 +32308,7 @@
       </c>
       <c r="J379" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K379" t="inlineStr">
@@ -32992,7 +32992,7 @@
       </c>
       <c r="J387" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K387" t="inlineStr">
@@ -33163,12 +33163,12 @@
       </c>
       <c r="J389" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K389" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L389" t="inlineStr">
@@ -33417,7 +33417,7 @@
       </c>
       <c r="J392" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K392" t="inlineStr">
@@ -33583,12 +33583,12 @@
       </c>
       <c r="J394" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K394" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L394" t="inlineStr">
@@ -33759,7 +33759,7 @@
       </c>
       <c r="J396" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K396" t="inlineStr">
@@ -33847,12 +33847,12 @@
       </c>
       <c r="J397" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K397" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L397" t="inlineStr">
@@ -34101,12 +34101,12 @@
       </c>
       <c r="J400" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K400" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L400" t="inlineStr">
@@ -34277,7 +34277,7 @@
       </c>
       <c r="J402" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K402" t="inlineStr">
@@ -34365,12 +34365,12 @@
       </c>
       <c r="J403" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K403" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L403" t="inlineStr">
@@ -34453,12 +34453,12 @@
       </c>
       <c r="J404" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K404" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L404" t="inlineStr">
@@ -34541,7 +34541,7 @@
       </c>
       <c r="J405" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K405" t="inlineStr">
@@ -34629,12 +34629,12 @@
       </c>
       <c r="J406" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K406" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L406" t="inlineStr">
@@ -34795,7 +34795,7 @@
       </c>
       <c r="J408" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K408" t="inlineStr">
@@ -35112,12 +35112,12 @@
       </c>
       <c r="J412" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K412" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L412" t="inlineStr">
@@ -35444,12 +35444,12 @@
       </c>
       <c r="J416" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K416" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L416" t="inlineStr">
@@ -35600,12 +35600,12 @@
       </c>
       <c r="J418" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K418" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L418" t="inlineStr">
@@ -35688,7 +35688,7 @@
       </c>
       <c r="J419" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K419" t="inlineStr">
@@ -35776,12 +35776,12 @@
       </c>
       <c r="J420" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K420" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L420" t="inlineStr">
@@ -35952,12 +35952,12 @@
       </c>
       <c r="J422" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K422" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L422" t="inlineStr">
@@ -36211,7 +36211,7 @@
       </c>
       <c r="K425" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L425" t="inlineStr">
@@ -36709,7 +36709,7 @@
       </c>
       <c r="K431" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L431" t="inlineStr">
@@ -37310,12 +37310,12 @@
       </c>
       <c r="J438" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K438" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L438" t="inlineStr">
@@ -37398,12 +37398,12 @@
       </c>
       <c r="J439" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K439" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L439" t="inlineStr">
@@ -37700,12 +37700,12 @@
       </c>
       <c r="J443" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K443" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L443" t="inlineStr">
@@ -37788,12 +37788,12 @@
       </c>
       <c r="J444" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K444" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L444" t="inlineStr">
@@ -37876,12 +37876,12 @@
       </c>
       <c r="J445" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K445" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L445" t="inlineStr">
@@ -38301,12 +38301,12 @@
       </c>
       <c r="J450" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K450" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L450" t="inlineStr">
@@ -38389,12 +38389,12 @@
       </c>
       <c r="J451" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K451" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L451" t="inlineStr">
@@ -38477,12 +38477,12 @@
       </c>
       <c r="J452" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K452" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L452" t="inlineStr">
@@ -38565,12 +38565,12 @@
       </c>
       <c r="J453" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K453" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L453" t="inlineStr">
@@ -38741,12 +38741,12 @@
       </c>
       <c r="J455" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K455" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L455" t="inlineStr">
@@ -38829,12 +38829,12 @@
       </c>
       <c r="J456" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K456" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L456" t="inlineStr">
@@ -38922,7 +38922,7 @@
       </c>
       <c r="K457" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L457" t="inlineStr">
@@ -39093,7 +39093,7 @@
       </c>
       <c r="J459" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K459" t="inlineStr">
@@ -39541,7 +39541,7 @@
       </c>
       <c r="J465" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K465" t="inlineStr">
@@ -39697,12 +39697,12 @@
       </c>
       <c r="J467" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K467" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L467" t="inlineStr">
@@ -39873,12 +39873,12 @@
       </c>
       <c r="J469" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K469" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L469" t="inlineStr">
@@ -39961,7 +39961,7 @@
       </c>
       <c r="J470" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K470" t="inlineStr">
@@ -40049,12 +40049,12 @@
       </c>
       <c r="J471" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K471" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L471" t="inlineStr">
@@ -40137,12 +40137,12 @@
       </c>
       <c r="J472" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K472" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L472" t="inlineStr">
@@ -40313,12 +40313,12 @@
       </c>
       <c r="J474" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K474" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L474" t="inlineStr">
@@ -40401,7 +40401,7 @@
       </c>
       <c r="J475" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K475" t="inlineStr">
@@ -40489,12 +40489,12 @@
       </c>
       <c r="J476" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K476" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L476" t="inlineStr">
@@ -40884,7 +40884,7 @@
       </c>
       <c r="K481" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L481" t="inlineStr">
@@ -41098,7 +41098,7 @@
       </c>
       <c r="J484" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K484" t="inlineStr">
@@ -41450,12 +41450,12 @@
       </c>
       <c r="J488" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K488" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L488" t="inlineStr">
@@ -41626,12 +41626,12 @@
       </c>
       <c r="J490" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K490" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L490" t="inlineStr">
@@ -41709,12 +41709,12 @@
       </c>
       <c r="J491" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K491" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L491" t="inlineStr">
@@ -42129,12 +42129,12 @@
       </c>
       <c r="J496" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K496" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L496" t="inlineStr">
@@ -42217,12 +42217,12 @@
       </c>
       <c r="J497" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K497" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L497" t="inlineStr">
@@ -42305,12 +42305,12 @@
       </c>
       <c r="J498" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K498" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L498" t="inlineStr">
@@ -42662,7 +42662,7 @@
       </c>
       <c r="K502" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L502" t="inlineStr">
@@ -42833,12 +42833,12 @@
       </c>
       <c r="J504" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K504" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L504" t="inlineStr">
@@ -43014,7 +43014,7 @@
       </c>
       <c r="K506" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L506" t="inlineStr">
@@ -43756,12 +43756,12 @@
       </c>
       <c r="J515" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K515" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L515" t="inlineStr">
@@ -43844,12 +43844,12 @@
       </c>
       <c r="J516" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K516" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L516" t="inlineStr">
@@ -43932,12 +43932,12 @@
       </c>
       <c r="J517" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K517" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L517" t="inlineStr">
@@ -44020,12 +44020,12 @@
       </c>
       <c r="J518" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K518" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L518" t="inlineStr">
@@ -44548,12 +44548,12 @@
       </c>
       <c r="J524" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K524" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L524" t="inlineStr">
@@ -44636,12 +44636,12 @@
       </c>
       <c r="J525" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K525" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L525" t="inlineStr">
@@ -44978,12 +44978,12 @@
       </c>
       <c r="J529" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K529" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L529" t="inlineStr">
@@ -45154,12 +45154,12 @@
       </c>
       <c r="J531" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K531" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L531" t="inlineStr">
@@ -45242,12 +45242,12 @@
       </c>
       <c r="J532" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K532" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L532" t="inlineStr">
@@ -45496,12 +45496,12 @@
       </c>
       <c r="J535" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K535" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L535" t="inlineStr">
@@ -45755,7 +45755,7 @@
       </c>
       <c r="J538" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K538" t="inlineStr">
@@ -45931,12 +45931,12 @@
       </c>
       <c r="J540" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K540" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L540" t="inlineStr">
@@ -46439,12 +46439,12 @@
       </c>
       <c r="J546" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K546" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L546" t="inlineStr">
@@ -46615,12 +46615,12 @@
       </c>
       <c r="J548" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K548" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L548" t="inlineStr">
@@ -46879,12 +46879,12 @@
       </c>
       <c r="J551" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K551" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L551" t="inlineStr">
@@ -47055,12 +47055,12 @@
       </c>
       <c r="J553" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K553" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L553" t="inlineStr">
@@ -47143,12 +47143,12 @@
       </c>
       <c r="J554" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K554" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L554" t="inlineStr">
@@ -47309,12 +47309,12 @@
       </c>
       <c r="J556" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K556" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L556" t="inlineStr">
@@ -47397,12 +47397,12 @@
       </c>
       <c r="J557" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K557" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L557" t="inlineStr">
@@ -47822,12 +47822,12 @@
       </c>
       <c r="J562" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K562" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L562" t="inlineStr">
@@ -47910,12 +47910,12 @@
       </c>
       <c r="J563" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K563" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L563" t="inlineStr">
@@ -47998,12 +47998,12 @@
       </c>
       <c r="J564" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K564" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L564" t="inlineStr">
@@ -48086,12 +48086,12 @@
       </c>
       <c r="J565" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K565" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L565" t="inlineStr">
@@ -48672,12 +48672,12 @@
       </c>
       <c r="J572" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K572" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L572" t="inlineStr">
@@ -48760,12 +48760,12 @@
       </c>
       <c r="J573" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K573" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L573" t="inlineStr">
@@ -49102,12 +49102,12 @@
       </c>
       <c r="J577" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K577" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L577" t="inlineStr">
@@ -49190,12 +49190,12 @@
       </c>
       <c r="J578" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K578" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L578" t="inlineStr">
@@ -49278,7 +49278,7 @@
       </c>
       <c r="J579" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K579" t="inlineStr">
@@ -49366,12 +49366,12 @@
       </c>
       <c r="J580" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K580" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L580" t="inlineStr">
@@ -49972,12 +49972,12 @@
       </c>
       <c r="J587" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K587" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L587" t="inlineStr">
@@ -50060,12 +50060,12 @@
       </c>
       <c r="J588" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K588" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L588" t="inlineStr">
@@ -50314,12 +50314,12 @@
       </c>
       <c r="J591" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K591" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L591" t="inlineStr">
@@ -50490,12 +50490,12 @@
       </c>
       <c r="J593" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K593" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L593" t="inlineStr">
@@ -50578,12 +50578,12 @@
       </c>
       <c r="J594" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K594" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L594" t="inlineStr">
@@ -50754,12 +50754,12 @@
       </c>
       <c r="J596" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K596" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L596" t="inlineStr">
@@ -50842,12 +50842,12 @@
       </c>
       <c r="J597" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K597" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L597" t="inlineStr">
@@ -50930,12 +50930,12 @@
       </c>
       <c r="J598" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K598" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L598" t="inlineStr">
@@ -51018,12 +51018,12 @@
       </c>
       <c r="J599" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K599" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L599" t="inlineStr">
@@ -51448,7 +51448,7 @@
       </c>
       <c r="J604" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K604" t="inlineStr">
@@ -51614,12 +51614,12 @@
       </c>
       <c r="J606" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K606" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L606" t="inlineStr">
@@ -51780,12 +51780,12 @@
       </c>
       <c r="J608" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K608" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L608" t="inlineStr">
@@ -52038,7 +52038,7 @@
       </c>
       <c r="J611" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K611" t="inlineStr">
@@ -52219,7 +52219,7 @@
       </c>
       <c r="K613" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L613" t="inlineStr">
@@ -52380,12 +52380,12 @@
       </c>
       <c r="J615" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K615" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L615" t="inlineStr">
@@ -52468,7 +52468,7 @@
       </c>
       <c r="J616" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K616" t="inlineStr">
@@ -53122,12 +53122,12 @@
       </c>
       <c r="J624" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K624" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L624" t="inlineStr">
@@ -53210,12 +53210,12 @@
       </c>
       <c r="J625" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K625" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L625" t="inlineStr">
@@ -53298,12 +53298,12 @@
       </c>
       <c r="J626" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K626" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L626" t="inlineStr">
@@ -53386,12 +53386,12 @@
       </c>
       <c r="J627" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K627" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L627" t="inlineStr">
@@ -53474,12 +53474,12 @@
       </c>
       <c r="J628" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K628" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L628" t="inlineStr">
@@ -53894,12 +53894,12 @@
       </c>
       <c r="J633" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K633" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L633" t="inlineStr">
@@ -54366,12 +54366,12 @@
       </c>
       <c r="J639" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K639" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L639" t="inlineStr">
@@ -54532,12 +54532,12 @@
       </c>
       <c r="J641" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K641" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L641" t="inlineStr">
@@ -54942,12 +54942,12 @@
       </c>
       <c r="J646" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K646" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L646" t="inlineStr">
@@ -55030,12 +55030,12 @@
       </c>
       <c r="J647" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K647" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L647" t="inlineStr">
@@ -55118,7 +55118,7 @@
       </c>
       <c r="J648" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K648" t="inlineStr">
@@ -55284,7 +55284,7 @@
       </c>
       <c r="J650" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K650" t="inlineStr">
@@ -55460,12 +55460,12 @@
       </c>
       <c r="J652" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K652" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L652" t="inlineStr">
@@ -55704,12 +55704,12 @@
       </c>
       <c r="J655" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="K655" t="inlineStr">
         <is>
-          <t>JV</t>
+          <t>Junior Varsity</t>
         </is>
       </c>
       <c r="L655" t="inlineStr">

</xml_diff>